<commit_message>
PLC.PROG cleaned ad refactored
</commit_message>
<xml_diff>
--- a/Warehouse Manager/Defaults/Components_default.xlsx
+++ b/Warehouse Manager/Defaults/Components_default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\Warehouse\Warehouse Manager\Defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454D89BD-8DCD-4771-AD0B-361FE7888B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F90E3B-E90C-48F6-B669-51BC718D0333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5976" yWindow="0" windowWidth="17064" windowHeight="10188" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slots" sheetId="5" r:id="rId1"/>
@@ -306,7 +306,22 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -491,7 +506,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{21235CA6-5A0E-49B8-ADBE-3BBEC2EA356F}" name="Tabella4" displayName="Tabella4" ref="A1:O1001" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{21235CA6-5A0E-49B8-ADBE-3BBEC2EA356F}" name="Tabella4" displayName="Tabella4" ref="A1:O1001" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:O1001" xr:uid="{21235CA6-5A0E-49B8-ADBE-3BBEC2EA356F}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{881521F8-3A36-403A-89CF-3FD2899697C0}" name="ID"/>
@@ -515,10 +530,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A040AAC6-FB7A-4F73-AFA3-B11D4C09CA39}" name="Tabella2" displayName="Tabella2" ref="A1:F21" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A040AAC6-FB7A-4F73-AFA3-B11D4C09CA39}" name="Tabella2" displayName="Tabella2" ref="A1:F21" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:F21" xr:uid="{A040AAC6-FB7A-4F73-AFA3-B11D4C09CA39}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C560BA8C-A555-495D-AA48-207B749EC290}" name="Enumeration"/>
+    <tableColumn id="1" xr3:uid="{C560BA8C-A555-495D-AA48-207B749EC290}" name="Enumeration" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{4631A140-5AE9-4AF7-BDC5-C24BB348B7A0}" name="Slot State"/>
     <tableColumn id="3" xr3:uid="{73C6846B-429D-4FD9-866F-E9F0B75064E2}" name="Container State"/>
     <tableColumn id="4" xr3:uid="{A34CB157-5654-4EF7-B8C0-B40175E9B729}" name="Plc State"/>
@@ -530,11 +545,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C4A7254-44FD-4CE5-A225-24871254660C}" name="Tabella1" displayName="Tabella1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C4A7254-44FD-4CE5-A225-24871254660C}" name="Tabella1" displayName="Tabella1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:B6" xr:uid="{7C4A7254-44FD-4CE5-A225-24871254660C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{79B85F13-9548-441C-9C42-BA34894E18C2}" name="Dimension" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{73D0EE91-BBD3-48E8-91DA-2AC84D3D1B14}" name="Unit" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{79B85F13-9548-441C-9C42-BA34894E18C2}" name="Dimension" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{73D0EE91-BBD3-48E8-91DA-2AC84D3D1B14}" name="Unit" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -839,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624E8E99-32C2-4C33-8CFB-BBA118DF1C3A}">
   <dimension ref="A1:Q201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E185" sqref="E185:E201"/>
     </sheetView>
   </sheetViews>
@@ -20609,8 +20624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20645,7 +20660,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -20668,7 +20683,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -20691,7 +20706,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="D4" t="s">
@@ -20705,7 +20720,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="I5" t="s">
@@ -20713,7 +20728,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="I6" t="s">
@@ -20721,7 +20736,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -20741,7 +20756,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="C8" t="s">
@@ -20752,7 +20767,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="C9" t="s">
@@ -20760,17 +20775,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -20793,7 +20808,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="D13" t="s">
@@ -20804,22 +20819,22 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -20836,29 +20851,30 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -21164,20 +21180,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0786a6a0-d0ce-491c-9482-af6677a0782d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0786a6a0-d0ce-491c-9482-af6677a0782d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21200,14 +21216,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37253E60-5741-402B-A9E0-4CDD3515F96E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A118553A-38E2-4959-9596-49A9A985FBAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -21222,4 +21230,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37253E60-5741-402B-A9E0-4CDD3515F96E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>